<commit_message>
Inital commit of results panel
</commit_message>
<xml_diff>
--- a/GUI Layout.xlsx
+++ b/GUI Layout.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hickey.221\Documents\GitHub\Alchromy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rich\Documents\GitHub\Alchromy\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E25D9E-CFBF-4D06-AD92-CD7DECCC2586}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26685" windowHeight="10050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26685" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Input files</t>
   </si>
@@ -95,9 +97,6 @@
     <t>[List select]</t>
   </si>
   <si>
-    <t>Operator ID</t>
-  </si>
-  <si>
     <t>[GO]</t>
   </si>
   <si>
@@ -114,12 +113,45 @@
   </si>
   <si>
     <t>Verbobse debug output</t>
+  </si>
+  <si>
+    <t>File note</t>
+  </si>
+  <si>
+    <t>Plot</t>
+  </si>
+  <si>
+    <t>[File or dir name]</t>
+  </si>
+  <si>
+    <t>Results of run:</t>
+  </si>
+  <si>
+    <t>Dataset:</t>
+  </si>
+  <si>
+    <t>[Dropdown list]</t>
+  </si>
+  <si>
+    <t>Species:</t>
+  </si>
+  <si>
+    <t>Scrollable list</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>Open new .alch file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,7 +193,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -236,8 +268,140 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
-      <top style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -250,7 +414,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -262,10 +426,23 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -277,8 +454,53 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -287,13 +509,24 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -302,53 +535,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right style="double">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -365,37 +553,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -404,130 +562,110 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -543,74 +681,92 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -892,11 +1048,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,37 +1096,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="11"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="25"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="27" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -986,21 +1142,21 @@
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="J3" s="28"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1014,13 +1170,13 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="13"/>
+      <c r="J4" s="28"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -1034,16 +1190,16 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="13"/>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -1056,23 +1212,23 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="13"/>
+      <c r="J6" s="28"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="E7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1080,49 +1236,49 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="13"/>
+      <c r="J7" s="28"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="33"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="31"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>29</v>
+      <c r="E9" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>11</v>
@@ -1130,32 +1286,33 @@
       <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="34"/>
+      <c r="H9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="35"/>
-    </row>
+      <c r="E10" s="33"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="37"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="H9:J10"/>
@@ -1165,5 +1322,213 @@
     <mergeCell ref="E2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A88CEA-FA6B-4883-913C-A2D6D32B50E5}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="50"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="42"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="43"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="43"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="43"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="52"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="42"/>
+      <c r="J7" s="43"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="52"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="43"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="44"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="46"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:B8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>